<commit_message>
Add day 2 files
</commit_message>
<xml_diff>
--- a/lab_06/data/lab_data.xlsx
+++ b/lab_06/data/lab_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kavidey/Sync/Mudd/FA24/E157/lab_06/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9FBA0F-4C1F-8C4E-BBC1-6822B1FF1155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F30BF5-8AA8-F248-9800-648D9FF22718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{222885BB-60D2-074B-9533-30A0874E1DCF}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{222885BB-60D2-074B-9533-30A0874E1DCF}"/>
   </bookViews>
   <sheets>
     <sheet name="sweep_time" sheetId="1" r:id="rId1"/>
     <sheet name="one_tone" sheetId="2" r:id="rId2"/>
     <sheet name="two_tone" sheetId="3" r:id="rId3"/>
+    <sheet name="two_tone_double" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Sweep Time [ms]</t>
   </si>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>VBW [Hz]</t>
+  </si>
+  <si>
+    <t>Attenuation [dB]</t>
   </si>
 </sst>
 </file>
@@ -434,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8282264-B1F0-7540-B6D2-63AE2E742FB2}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="182" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -789,8 +793,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77AA2870-9CD6-B945-B92F-2217986FA3CB}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView zoomScale="214" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -802,7 +806,9 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -811,7 +817,9 @@
       <c r="B2" s="1">
         <v>-77.5</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -820,7 +828,9 @@
       <c r="B3" s="1">
         <v>-67.7</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -829,7 +839,9 @@
       <c r="B4" s="1">
         <v>-57.5</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -838,7 +850,9 @@
       <c r="B5" s="1">
         <v>-47.6</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -847,7 +861,9 @@
       <c r="B6" s="1">
         <v>-37.4</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -856,7 +872,9 @@
       <c r="B7" s="1">
         <v>-27.36</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -865,7 +883,9 @@
       <c r="B8" s="1">
         <v>-19.5</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -874,7 +894,9 @@
       <c r="B9" s="1">
         <v>-17.55</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -883,7 +905,9 @@
       <c r="B10" s="1">
         <v>-16.62</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -892,7 +916,9 @@
       <c r="B11" s="1">
         <v>-15.71</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -901,7 +927,9 @@
       <c r="B12" s="1">
         <v>-14.81</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -910,7 +938,9 @@
       <c r="B13" s="1">
         <v>-13.88</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -919,7 +949,9 @@
       <c r="B14" s="1">
         <v>-13.14</v>
       </c>
-      <c r="C14" s="1"/>
+      <c r="C14" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -928,7 +960,9 @@
       <c r="B15" s="1">
         <v>-12.51</v>
       </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -937,207 +971,517 @@
       <c r="B16" s="1">
         <v>-12.04</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="1">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA1BF22D-CEA2-A34E-9FAF-1F0B859FE165}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K1" activeCellId="6" sqref="A1:B1 C1 D1 H1 I1 J1 K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1">
         <v>600</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>601</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>1200</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>1201</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>1202</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>1800</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>1801</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>1802</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>1803</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>-58</v>
       </c>
       <c r="B2" s="1">
-        <v>-60.5</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1">
         <v>-60.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D2" s="1">
+        <v>-60.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>-48</v>
       </c>
       <c r="B3" s="1">
-        <v>-50.5</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
         <v>-50.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D3" s="1">
+        <v>-50.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>-38</v>
       </c>
       <c r="B4" s="1">
-        <v>-40.6</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
         <v>-40.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D4" s="1">
+        <v>-40.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>-28</v>
       </c>
       <c r="B5" s="1">
-        <v>-30.5</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1">
         <v>-30.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D5" s="1">
+        <v>-30.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
+        <v>-25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="H6" s="1">
+        <v>-73.7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-63.63</v>
+      </c>
+      <c r="J6" s="1">
+        <v>-63.6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>-73.400000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>-23</v>
       </c>
+      <c r="B7" s="1">
+        <v>30</v>
+      </c>
+      <c r="E7" s="1">
+        <v>-72.72</v>
+      </c>
+      <c r="F7" s="1">
+        <v>-65.81</v>
+      </c>
+      <c r="G7" s="1">
+        <v>-75.540000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>-22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="H8" s="1">
+        <v>-64.099999999999994</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-54.6</v>
+      </c>
+      <c r="J8" s="1">
+        <v>-54.5</v>
+      </c>
+      <c r="K8" s="1">
+        <v>-63.59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>-21</v>
+      </c>
+      <c r="B9" s="1">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-66.849999999999994</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-61.11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>-66.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>-20</v>
+      </c>
+      <c r="B10" s="1">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>-57.5</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-48.5</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-48.3</v>
+      </c>
+      <c r="K10" s="1">
+        <v>-56.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>-20</v>
+      </c>
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-22.6</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-22.6</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-63.4</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-58.4</v>
+      </c>
+      <c r="G11" s="1">
+        <v>-64.599999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>-19</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>-53</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-45</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-44</v>
+      </c>
+      <c r="K12" s="1">
+        <v>-53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>-19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-62.51</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-56.65</v>
+      </c>
+      <c r="G13" s="1">
+        <v>-62.3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-73</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-65.89</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-65.37</v>
+      </c>
+      <c r="K13" s="1">
+        <v>-73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>-18</v>
+      </c>
+      <c r="B14" s="1">
+        <v>30</v>
+      </c>
+      <c r="C14" s="1">
+        <v>-20.8</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-20.8</v>
+      </c>
+      <c r="E14" s="1">
+        <v>-60.68</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-54.36</v>
+      </c>
+      <c r="G14" s="1">
+        <v>-60.64</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-70.36</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-61.31</v>
+      </c>
+      <c r="J14" s="1">
+        <v>-61.3</v>
+      </c>
+      <c r="K14" s="1">
+        <v>-68.89</v>
+      </c>
+    </row>
+    <row r="21" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADCD384-8081-C348-9134-20EEBDDCF9FF}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1">
+        <v>600</v>
+      </c>
+      <c r="D1">
+        <v>601</v>
+      </c>
+      <c r="E1">
+        <v>1800</v>
+      </c>
+      <c r="F1">
+        <v>1801</v>
+      </c>
+      <c r="G1">
+        <v>1802</v>
+      </c>
+      <c r="H1">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>-50</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>-16</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-15.91</v>
+      </c>
+      <c r="E2" s="1">
+        <v>-44.1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>-31.7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>-31.6</v>
+      </c>
+      <c r="H2" s="1">
+        <v>-43.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>-53</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1">
+        <v>-16.95</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-16.600000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>-46.12</v>
+      </c>
+      <c r="F3" s="1">
+        <v>-38.200000000000003</v>
+      </c>
+      <c r="G3" s="1">
+        <v>-38.1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>-45.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>-55</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>-18.079999999999998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-18.010000000000002</v>
+      </c>
+      <c r="E4" s="1">
+        <v>-53.3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>-45.8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>-46.8</v>
+      </c>
+      <c r="H4" s="1">
+        <v>-53.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>-57</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <v>-19.66</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-19.57</v>
+      </c>
+      <c r="E5" s="1">
+        <v>-61.4</v>
+      </c>
+      <c r="F5" s="1">
+        <v>-53.6</v>
+      </c>
+      <c r="G5" s="1">
+        <v>-53.9</v>
+      </c>
+      <c r="H5" s="1">
+        <v>-62.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>-58.2</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-20.74</v>
+      </c>
       <c r="D6" s="1">
-        <v>-72.72</v>
+        <v>-20.66</v>
       </c>
       <c r="E6" s="1">
-        <v>-65.81</v>
+        <v>-66.569999999999993</v>
       </c>
       <c r="F6" s="1">
-        <v>-75.540000000000006</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>-21</v>
-      </c>
-      <c r="D7" s="1">
-        <v>-66.849999999999994</v>
-      </c>
-      <c r="E7" s="1">
-        <v>-61.11</v>
-      </c>
-      <c r="F7" s="1">
+        <v>-58.3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>-58.5</v>
+      </c>
+      <c r="H6" s="1">
         <v>-66.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>-20</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-22.6</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-22.6</v>
-      </c>
-      <c r="D8" s="1">
-        <v>-63.4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>-58.4</v>
-      </c>
-      <c r="F8" s="1">
-        <v>-64.599999999999994</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>-19</v>
-      </c>
-      <c r="D9" s="1">
-        <v>-62.51</v>
-      </c>
-      <c r="E9" s="1">
-        <v>-56.65</v>
-      </c>
-      <c r="F9" s="1">
-        <v>-62.3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>-73</v>
-      </c>
-      <c r="H9" s="1">
-        <v>-65.89</v>
-      </c>
-      <c r="I9" s="1">
-        <v>-65.37</v>
-      </c>
-      <c r="J9" s="1">
-        <v>-73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>-18</v>
-      </c>
-      <c r="B10" s="1">
-        <v>-20.8</v>
-      </c>
-      <c r="C10" s="1">
-        <v>-20.8</v>
-      </c>
-      <c r="D10" s="1">
-        <v>-60.68</v>
-      </c>
-      <c r="E10" s="1">
-        <v>-54.36</v>
-      </c>
-      <c r="F10" s="1">
-        <v>-60.64</v>
-      </c>
-      <c r="G10" s="1">
-        <v>-70.36</v>
-      </c>
-      <c r="H10" s="1">
-        <v>-61.31</v>
-      </c>
-      <c r="I10" s="1">
-        <v>-61.3</v>
-      </c>
-      <c r="J10" s="1">
-        <v>-68.89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add finished data and code for lab 6
</commit_message>
<xml_diff>
--- a/lab_06/data/lab_data.xlsx
+++ b/lab_06/data/lab_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kavidey/Sync/Mudd/FA24/E157/lab_06/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F30BF5-8AA8-F248-9800-648D9FF22718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00702D4F-06E6-5741-9645-77027750C71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="3" xr2:uid="{222885BB-60D2-074B-9533-30A0874E1DCF}"/>
   </bookViews>
@@ -1315,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ADCD384-8081-C348-9134-20EEBDDCF9FF}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1355,131 +1355,105 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>-50</v>
+        <v>-53</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C2" s="1">
-        <v>-16</v>
+        <v>-16.95</v>
       </c>
       <c r="D2" s="1">
-        <v>-15.91</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="E2" s="1">
-        <v>-44.1</v>
+        <v>-46.12</v>
       </c>
       <c r="F2" s="1">
-        <v>-31.7</v>
+        <v>-38.200000000000003</v>
       </c>
       <c r="G2" s="1">
-        <v>-31.6</v>
+        <v>-38.1</v>
       </c>
       <c r="H2" s="1">
-        <v>-43.5</v>
+        <v>-45.9</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>-53</v>
+        <v>-55</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1">
-        <v>-16.95</v>
+        <v>-18.079999999999998</v>
       </c>
       <c r="D3" s="1">
-        <v>-16.600000000000001</v>
+        <v>-18.010000000000002</v>
       </c>
       <c r="E3" s="1">
-        <v>-46.12</v>
+        <v>-53.3</v>
       </c>
       <c r="F3" s="1">
-        <v>-38.200000000000003</v>
+        <v>-45.8</v>
       </c>
       <c r="G3" s="1">
-        <v>-38.1</v>
+        <v>-46.8</v>
       </c>
       <c r="H3" s="1">
-        <v>-45.9</v>
+        <v>-53.1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>-55</v>
+        <v>-57</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1">
-        <v>-18.079999999999998</v>
+        <v>-19.66</v>
       </c>
       <c r="D4" s="1">
-        <v>-18.010000000000002</v>
+        <v>-19.57</v>
       </c>
       <c r="E4" s="1">
-        <v>-53.3</v>
+        <v>-61.4</v>
       </c>
       <c r="F4" s="1">
-        <v>-45.8</v>
+        <v>-53.6</v>
       </c>
       <c r="G4" s="1">
-        <v>-46.8</v>
+        <v>-53.9</v>
       </c>
       <c r="H4" s="1">
-        <v>-53.1</v>
+        <v>-62.2</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>-57</v>
+        <v>-58.2</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1">
-        <v>-19.66</v>
+        <v>-20.74</v>
       </c>
       <c r="D5" s="1">
-        <v>-19.57</v>
+        <v>-20.66</v>
       </c>
       <c r="E5" s="1">
-        <v>-61.4</v>
+        <v>-66.569999999999993</v>
       </c>
       <c r="F5" s="1">
-        <v>-53.6</v>
+        <v>-58.3</v>
       </c>
       <c r="G5" s="1">
-        <v>-53.9</v>
+        <v>-58.5</v>
       </c>
       <c r="H5" s="1">
-        <v>-62.2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>-58.2</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>-20.74</v>
-      </c>
-      <c r="D6" s="1">
-        <v>-20.66</v>
-      </c>
-      <c r="E6" s="1">
-        <v>-66.569999999999993</v>
-      </c>
-      <c r="F6" s="1">
-        <v>-58.3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>-58.5</v>
-      </c>
-      <c r="H6" s="1">
         <v>-66.5</v>
       </c>
     </row>

</xml_diff>